<commit_message>
feat: Add signature image to document
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/rental-support-application.xlsx
+++ b/src/main/resources/templates/rental-support-application.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/1000bang/vacation/api/src/main/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ACC4DF8-E509-2B44-BD3D-8D3E2263AB15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B62034BA-12C1-2C4A-B177-1301A0F85096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>신청 일자</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -241,6 +241,38 @@
       </rPr>
       <t>{{MONTH}}</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{DAM_SIG1}}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{DAM_SIG2}}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{TIM_SIG1}}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{TIM_SIG2}}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{BU_SIG1}}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{BU_SIG2}}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{DEA_SIG1}}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{DEA_SIG2}}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1234,7 +1266,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection activeCell="A6" sqref="A6:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
@@ -1293,10 +1325,18 @@
       <c r="C3" s="55"/>
       <c r="D3" s="56"/>
       <c r="E3" s="63"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="30"/>
+      <c r="F3" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3" s="30" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="4" spans="1:12" ht="28" customHeight="1">
       <c r="A4" s="1" t="s">
@@ -1323,10 +1363,18 @@
       <c r="C5" s="60"/>
       <c r="D5" s="61"/>
       <c r="E5" s="64"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="7"/>
+      <c r="F5" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="6" spans="1:12" ht="28" customHeight="1" thickTop="1">
       <c r="A6" s="65" t="s">

</xml_diff>